<commit_message>
fix filter for no streaming schedule
</commit_message>
<xml_diff>
--- a/docs/assets/docs/Schedule.xlsx
+++ b/docs/assets/docs/Schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3760" uniqueCount="2202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3763" uniqueCount="2202">
   <si>
     <t>id</t>
   </si>
@@ -37928,7 +37928,7 @@
         <v>44678.666666666664</v>
       </c>
       <c r="L1302" s="46">
-        <f t="shared" ref="L1302:L1354" si="50">(K1302-Date(1970,1,1))*86400*1000</f>
+        <f t="shared" ref="L1302:L1337" si="50">(K1302-Date(1970,1,1))*86400*1000</f>
         <v>1651075200000</v>
       </c>
     </row>
@@ -38784,752 +38784,791 @@
       </c>
     </row>
     <row r="1338">
-      <c r="A1338" s="1">
-        <v>1278.0</v>
-      </c>
+      <c r="A1338" s="1"/>
       <c r="B1338" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C1338" s="1" t="s">
-        <v>2154</v>
-      </c>
-      <c r="D1338" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K1338" s="47">
-        <v>44684.625</v>
-      </c>
-      <c r="L1338" s="46">
-        <f t="shared" si="50"/>
-        <v>1651590000000</v>
+        <v>66</v>
+      </c>
+      <c r="C1338" s="1"/>
+      <c r="D1338" s="1"/>
+      <c r="K1338" s="47"/>
+      <c r="L1338" s="46"/>
+      <c r="M1338" s="1">
+        <v>1277.0</v>
       </c>
     </row>
     <row r="1339">
-      <c r="A1339" s="1">
-        <v>1279.0</v>
-      </c>
+      <c r="A1339" s="1"/>
       <c r="B1339" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C1339" s="1" t="s">
-        <v>2155</v>
-      </c>
-      <c r="D1339" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K1339" s="47">
-        <v>44685.708333333336</v>
-      </c>
-      <c r="L1339" s="46">
-        <f t="shared" si="50"/>
-        <v>1651683600000</v>
+        <v>195</v>
+      </c>
+      <c r="C1339" s="1"/>
+      <c r="D1339" s="1"/>
+      <c r="K1339" s="47"/>
+      <c r="L1339" s="46"/>
+      <c r="M1339" s="1">
+        <v>1277.0</v>
       </c>
     </row>
     <row r="1340">
-      <c r="A1340" s="1">
-        <v>1280.0</v>
-      </c>
+      <c r="A1340" s="1"/>
       <c r="B1340" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C1340" s="1" t="s">
-        <v>2156</v>
-      </c>
-      <c r="D1340" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K1340" s="47">
-        <v>44686.625</v>
-      </c>
-      <c r="L1340" s="46">
-        <f t="shared" si="50"/>
-        <v>1651762800000</v>
+        <v>215</v>
+      </c>
+      <c r="C1340" s="1"/>
+      <c r="D1340" s="1"/>
+      <c r="K1340" s="47"/>
+      <c r="L1340" s="46"/>
+      <c r="M1340" s="1">
+        <v>1277.0</v>
       </c>
     </row>
     <row r="1341">
       <c r="A1341" s="1">
-        <v>1281.0</v>
+        <v>1278.0</v>
       </c>
       <c r="B1341" s="1" t="s">
         <v>318</v>
       </c>
       <c r="C1341" s="1" t="s">
-        <v>2157</v>
+        <v>2154</v>
       </c>
       <c r="D1341" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K1341" s="47">
-        <v>44687.625</v>
+        <v>44684.625</v>
       </c>
       <c r="L1341" s="46">
-        <f t="shared" si="50"/>
-        <v>1651849200000</v>
+        <f t="shared" ref="L1341:L1357" si="51">(K1341-Date(1970,1,1))*86400*1000</f>
+        <v>1651590000000</v>
       </c>
     </row>
     <row r="1342">
       <c r="A1342" s="1">
-        <v>1282.0</v>
+        <v>1279.0</v>
       </c>
       <c r="B1342" s="1" t="s">
         <v>318</v>
       </c>
       <c r="C1342" s="1" t="s">
-        <v>2158</v>
+        <v>2155</v>
       </c>
       <c r="D1342" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K1342" s="47">
-        <v>44688.541666666664</v>
+        <v>44685.708333333336</v>
       </c>
       <c r="L1342" s="46">
-        <f t="shared" si="50"/>
-        <v>1651928400000</v>
+        <f t="shared" si="51"/>
+        <v>1651683600000</v>
       </c>
     </row>
     <row r="1343">
       <c r="A1343" s="1">
-        <v>1283.0</v>
+        <v>1280.0</v>
       </c>
       <c r="B1343" s="1" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="C1343" s="1" t="s">
-        <v>2159</v>
-      </c>
-      <c r="E1343" s="6" t="s">
-        <v>2160</v>
+        <v>2156</v>
+      </c>
+      <c r="D1343" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="K1343" s="47">
-        <v>44683.5</v>
+        <v>44686.625</v>
       </c>
       <c r="L1343" s="46">
-        <f t="shared" si="50"/>
-        <v>1651492800000</v>
+        <f t="shared" si="51"/>
+        <v>1651762800000</v>
       </c>
     </row>
     <row r="1344">
       <c r="A1344" s="1">
-        <v>1284.0</v>
+        <v>1281.0</v>
       </c>
       <c r="B1344" s="1" t="s">
-        <v>78</v>
+        <v>318</v>
       </c>
       <c r="C1344" s="1" t="s">
-        <v>2161</v>
+        <v>2157</v>
       </c>
       <c r="D1344" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E1344" s="6" t="s">
-        <v>2162</v>
-      </c>
       <c r="K1344" s="47">
-        <v>44682.791666666664</v>
+        <v>44687.625</v>
       </c>
       <c r="L1344" s="46">
-        <f t="shared" si="50"/>
-        <v>1651431600000</v>
+        <f t="shared" si="51"/>
+        <v>1651849200000</v>
       </c>
     </row>
     <row r="1345">
       <c r="A1345" s="1">
-        <v>1285.0</v>
+        <v>1282.0</v>
       </c>
       <c r="B1345" s="1" t="s">
-        <v>55</v>
+        <v>318</v>
       </c>
       <c r="C1345" s="1" t="s">
-        <v>2163</v>
+        <v>2158</v>
       </c>
       <c r="D1345" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E1345" s="6" t="s">
-        <v>2164</v>
-      </c>
       <c r="K1345" s="47">
-        <v>44683.541666666664</v>
+        <v>44688.541666666664</v>
       </c>
       <c r="L1345" s="46">
-        <f t="shared" si="50"/>
-        <v>1651496400000</v>
+        <f t="shared" si="51"/>
+        <v>1651928400000</v>
       </c>
     </row>
     <row r="1346">
       <c r="A1346" s="1">
-        <v>1286.0</v>
+        <v>1283.0</v>
       </c>
       <c r="B1346" s="1" t="s">
-        <v>55</v>
+        <v>333</v>
       </c>
       <c r="C1346" s="1" t="s">
-        <v>2165</v>
-      </c>
-      <c r="D1346" s="1" t="b">
-        <v>1</v>
+        <v>2159</v>
+      </c>
+      <c r="E1346" s="6" t="s">
+        <v>2160</v>
       </c>
       <c r="K1346" s="47">
-        <v>44684.458333333336</v>
+        <v>44683.5</v>
       </c>
       <c r="L1346" s="46">
-        <f t="shared" si="50"/>
-        <v>1651575600000</v>
+        <f t="shared" si="51"/>
+        <v>1651492800000</v>
       </c>
     </row>
     <row r="1347">
       <c r="A1347" s="1">
-        <v>1287.0</v>
+        <v>1284.0</v>
       </c>
       <c r="B1347" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="C1347" s="1" t="s">
-        <v>890</v>
+        <v>2161</v>
       </c>
       <c r="D1347" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="E1347" s="6" t="s">
+        <v>2162</v>
+      </c>
       <c r="K1347" s="47">
-        <v>44685.458333333336</v>
+        <v>44682.791666666664</v>
       </c>
       <c r="L1347" s="46">
-        <f t="shared" si="50"/>
-        <v>1651662000000</v>
+        <f t="shared" si="51"/>
+        <v>1651431600000</v>
       </c>
     </row>
     <row r="1348">
       <c r="A1348" s="1">
-        <v>1288.0</v>
+        <v>1285.0</v>
       </c>
       <c r="B1348" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C1348" s="1" t="s">
-        <v>2166</v>
+        <v>2163</v>
       </c>
       <c r="D1348" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="E1348" s="6" t="s">
+        <v>2164</v>
+      </c>
       <c r="K1348" s="47">
-        <v>44686.458333333336</v>
+        <v>44683.541666666664</v>
       </c>
       <c r="L1348" s="46">
-        <f t="shared" si="50"/>
-        <v>1651748400000</v>
+        <f t="shared" si="51"/>
+        <v>1651496400000</v>
       </c>
     </row>
     <row r="1349">
       <c r="A1349" s="1">
-        <v>1289.0</v>
+        <v>1286.0</v>
       </c>
       <c r="B1349" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C1349" s="1" t="s">
-        <v>2167</v>
+        <v>2165</v>
       </c>
       <c r="D1349" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K1349" s="47">
-        <v>44687.458333333336</v>
+        <v>44684.458333333336</v>
       </c>
       <c r="L1349" s="46">
-        <f t="shared" si="50"/>
-        <v>1651834800000</v>
+        <f t="shared" si="51"/>
+        <v>1651575600000</v>
       </c>
     </row>
     <row r="1350">
       <c r="A1350" s="1">
-        <v>1290.0</v>
+        <v>1287.0</v>
       </c>
       <c r="B1350" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C1350" s="1" t="s">
-        <v>1350</v>
+        <v>890</v>
       </c>
       <c r="D1350" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K1350" s="47">
-        <v>44688.5</v>
+        <v>44685.458333333336</v>
       </c>
       <c r="L1350" s="46">
-        <f t="shared" si="50"/>
-        <v>1651924800000</v>
+        <f t="shared" si="51"/>
+        <v>1651662000000</v>
       </c>
     </row>
     <row r="1351">
       <c r="A1351" s="1">
-        <v>1291.0</v>
+        <v>1288.0</v>
       </c>
       <c r="B1351" s="1" t="s">
-        <v>157</v>
+        <v>55</v>
       </c>
       <c r="C1351" s="1" t="s">
-        <v>2168</v>
+        <v>2166</v>
       </c>
       <c r="D1351" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E1351" s="6" t="s">
-        <v>2169</v>
-      </c>
       <c r="K1351" s="47">
-        <v>44682.541666666664</v>
+        <v>44686.458333333336</v>
       </c>
       <c r="L1351" s="46">
-        <f t="shared" si="50"/>
-        <v>1651410000000</v>
+        <f t="shared" si="51"/>
+        <v>1651748400000</v>
       </c>
     </row>
     <row r="1352">
       <c r="A1352" s="1">
-        <v>1292.0</v>
+        <v>1289.0</v>
       </c>
       <c r="B1352" s="1" t="s">
-        <v>157</v>
+        <v>55</v>
       </c>
       <c r="C1352" s="1" t="s">
-        <v>1940</v>
+        <v>2167</v>
       </c>
       <c r="D1352" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E1352" s="6" t="s">
-        <v>2170</v>
-      </c>
       <c r="K1352" s="47">
-        <v>44683.583333333336</v>
+        <v>44687.458333333336</v>
       </c>
       <c r="L1352" s="46">
-        <f t="shared" si="50"/>
-        <v>1651500000000</v>
+        <f t="shared" si="51"/>
+        <v>1651834800000</v>
       </c>
     </row>
     <row r="1353">
       <c r="A1353" s="1">
-        <v>1293.0</v>
+        <v>1290.0</v>
       </c>
       <c r="B1353" s="1" t="s">
-        <v>157</v>
+        <v>55</v>
       </c>
       <c r="C1353" s="1" t="s">
-        <v>2171</v>
+        <v>1350</v>
       </c>
       <c r="D1353" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K1353" s="47">
-        <v>44684.541666666664</v>
+        <v>44688.5</v>
       </c>
       <c r="L1353" s="46">
-        <f t="shared" si="50"/>
-        <v>1651582800000</v>
+        <f t="shared" si="51"/>
+        <v>1651924800000</v>
       </c>
     </row>
     <row r="1354">
       <c r="A1354" s="1">
-        <v>1294.0</v>
+        <v>1291.0</v>
       </c>
       <c r="B1354" s="1" t="s">
         <v>157</v>
       </c>
       <c r="C1354" s="1" t="s">
-        <v>2172</v>
+        <v>2168</v>
       </c>
       <c r="D1354" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="E1354" s="6" t="s">
+        <v>2169</v>
+      </c>
       <c r="K1354" s="47">
-        <v>44686.625</v>
+        <v>44682.541666666664</v>
       </c>
       <c r="L1354" s="46">
-        <f t="shared" si="50"/>
-        <v>1651762800000</v>
+        <f t="shared" si="51"/>
+        <v>1651410000000</v>
       </c>
     </row>
     <row r="1355">
-      <c r="A1355" s="1"/>
+      <c r="A1355" s="1">
+        <v>1292.0</v>
+      </c>
       <c r="B1355" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1355" s="1"/>
-      <c r="D1355" s="1"/>
-      <c r="K1355" s="47"/>
-      <c r="L1355" s="46"/>
-      <c r="M1355" s="1">
-        <v>1294.0</v>
+        <v>157</v>
+      </c>
+      <c r="C1355" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="D1355" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1355" s="6" t="s">
+        <v>2170</v>
+      </c>
+      <c r="K1355" s="47">
+        <v>44683.583333333336</v>
+      </c>
+      <c r="L1355" s="46">
+        <f t="shared" si="51"/>
+        <v>1651500000000</v>
       </c>
     </row>
     <row r="1356">
       <c r="A1356" s="1">
-        <v>1295.0</v>
+        <v>1293.0</v>
       </c>
       <c r="B1356" s="1" t="s">
         <v>157</v>
       </c>
       <c r="C1356" s="1" t="s">
-        <v>2173</v>
+        <v>2171</v>
       </c>
       <c r="D1356" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K1356" s="47">
-        <v>44687.5</v>
+        <v>44684.541666666664</v>
       </c>
       <c r="L1356" s="46">
-        <f t="shared" ref="L1356:L1360" si="51">(K1356-Date(1970,1,1))*86400*1000</f>
-        <v>1651838400000</v>
+        <f t="shared" si="51"/>
+        <v>1651582800000</v>
       </c>
     </row>
     <row r="1357">
       <c r="A1357" s="1">
-        <v>1296.0</v>
+        <v>1294.0</v>
       </c>
       <c r="B1357" s="1" t="s">
         <v>157</v>
       </c>
       <c r="C1357" s="1" t="s">
-        <v>2174</v>
+        <v>2172</v>
       </c>
       <c r="D1357" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K1357" s="47">
-        <v>44688.625</v>
+        <v>44686.625</v>
       </c>
       <c r="L1357" s="46">
         <f t="shared" si="51"/>
-        <v>1651935600000</v>
+        <v>1651762800000</v>
       </c>
     </row>
     <row r="1358">
-      <c r="A1358" s="1">
-        <v>1297.0</v>
-      </c>
+      <c r="A1358" s="1"/>
       <c r="B1358" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C1358" s="1" t="s">
-        <v>2175</v>
-      </c>
-      <c r="D1358" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E1358" s="6" t="s">
-        <v>2176</v>
-      </c>
-      <c r="K1358" s="47">
-        <v>44682.666666666664</v>
-      </c>
-      <c r="L1358" s="46">
-        <f t="shared" si="51"/>
-        <v>1651420800000</v>
+        <v>13</v>
+      </c>
+      <c r="C1358" s="1"/>
+      <c r="D1358" s="1"/>
+      <c r="K1358" s="47"/>
+      <c r="L1358" s="46"/>
+      <c r="M1358" s="1">
+        <v>1294.0</v>
       </c>
     </row>
     <row r="1359">
       <c r="A1359" s="1">
-        <v>1298.0</v>
+        <v>1295.0</v>
       </c>
       <c r="B1359" s="1" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="C1359" s="1" t="s">
-        <v>2177</v>
+        <v>2173</v>
       </c>
       <c r="D1359" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K1359" s="47">
-        <v>44692.958333333336</v>
+        <v>44687.5</v>
       </c>
       <c r="L1359" s="46">
-        <f t="shared" si="51"/>
-        <v>1652310000000</v>
+        <f t="shared" ref="L1359:L1363" si="52">(K1359-Date(1970,1,1))*86400*1000</f>
+        <v>1651838400000</v>
       </c>
     </row>
     <row r="1360">
       <c r="A1360" s="1">
-        <v>1299.0</v>
+        <v>1296.0</v>
       </c>
       <c r="B1360" s="1" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
       <c r="C1360" s="1" t="s">
-        <v>2178</v>
-      </c>
-      <c r="E1360" s="6" t="s">
-        <v>2179</v>
+        <v>2174</v>
+      </c>
+      <c r="D1360" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="K1360" s="47">
-        <v>44685.541666666664</v>
+        <v>44688.625</v>
       </c>
       <c r="L1360" s="46">
-        <f t="shared" si="51"/>
-        <v>1651669200000</v>
+        <f t="shared" si="52"/>
+        <v>1651935600000</v>
       </c>
     </row>
     <row r="1361">
       <c r="A1361" s="1">
-        <v>1300.0</v>
+        <v>1297.0</v>
       </c>
       <c r="B1361" s="1" t="s">
-        <v>286</v>
+        <v>146</v>
+      </c>
+      <c r="C1361" s="1" t="s">
+        <v>2175</v>
       </c>
       <c r="D1361" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="E1361" s="6" t="s">
+        <v>2176</v>
+      </c>
+      <c r="K1361" s="47">
+        <v>44682.666666666664</v>
+      </c>
+      <c r="L1361" s="46">
+        <f t="shared" si="52"/>
+        <v>1651420800000</v>
       </c>
     </row>
     <row r="1362">
       <c r="A1362" s="1">
-        <v>1301.0</v>
+        <v>1298.0</v>
       </c>
       <c r="B1362" s="1" t="s">
-        <v>13</v>
+        <v>146</v>
       </c>
       <c r="C1362" s="1" t="s">
-        <v>2180</v>
-      </c>
-      <c r="E1362" s="6" t="s">
-        <v>2181</v>
+        <v>2177</v>
+      </c>
+      <c r="D1362" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="K1362" s="47">
-        <v>44683.5</v>
+        <v>44692.958333333336</v>
       </c>
       <c r="L1362" s="46">
-        <f t="shared" ref="L1362:L1368" si="52">(K1362-Date(1970,1,1))*86400*1000</f>
-        <v>1651492800000</v>
+        <f t="shared" si="52"/>
+        <v>1652310000000</v>
       </c>
     </row>
     <row r="1363">
       <c r="A1363" s="1">
-        <v>1302.0</v>
+        <v>1299.0</v>
       </c>
       <c r="B1363" s="1" t="s">
-        <v>93</v>
+        <v>28</v>
       </c>
       <c r="C1363" s="1" t="s">
-        <v>2182</v>
+        <v>2178</v>
       </c>
       <c r="E1363" s="6" t="s">
-        <v>2042</v>
+        <v>2179</v>
       </c>
       <c r="K1363" s="47">
-        <v>44683.375</v>
+        <v>44685.541666666664</v>
       </c>
       <c r="L1363" s="46">
         <f t="shared" si="52"/>
-        <v>1651482000000</v>
+        <v>1651669200000</v>
       </c>
     </row>
     <row r="1364">
       <c r="A1364" s="1">
-        <v>1303.0</v>
+        <v>1300.0</v>
       </c>
       <c r="B1364" s="1" t="s">
-        <v>749</v>
-      </c>
-      <c r="C1364" s="1" t="s">
-        <v>2183</v>
+        <v>286</v>
       </c>
       <c r="D1364" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="K1364" s="47">
-        <v>44683.541666666664</v>
-      </c>
-      <c r="L1364" s="46">
-        <f t="shared" si="52"/>
-        <v>1651496400000</v>
       </c>
     </row>
     <row r="1365">
       <c r="A1365" s="1">
-        <v>1305.0</v>
+        <v>1301.0</v>
       </c>
       <c r="B1365" s="1" t="s">
-        <v>749</v>
+        <v>13</v>
       </c>
       <c r="C1365" s="1" t="s">
-        <v>2184</v>
-      </c>
-      <c r="D1365" s="1" t="b">
-        <v>1</v>
+        <v>2180</v>
+      </c>
+      <c r="E1365" s="6" t="s">
+        <v>2181</v>
       </c>
       <c r="K1365" s="47">
-        <v>44685.458333333336</v>
+        <v>44683.5</v>
       </c>
       <c r="L1365" s="46">
-        <f t="shared" si="52"/>
-        <v>1651662000000</v>
+        <f t="shared" ref="L1365:L1371" si="53">(K1365-Date(1970,1,1))*86400*1000</f>
+        <v>1651492800000</v>
       </c>
     </row>
     <row r="1366">
       <c r="A1366" s="1">
-        <v>1306.0</v>
+        <v>1302.0</v>
       </c>
       <c r="B1366" s="1" t="s">
-        <v>749</v>
+        <v>93</v>
       </c>
       <c r="C1366" s="1" t="s">
-        <v>2185</v>
-      </c>
-      <c r="D1366" s="1" t="b">
-        <v>1</v>
+        <v>2182</v>
+      </c>
+      <c r="E1366" s="6" t="s">
+        <v>2042</v>
       </c>
       <c r="K1366" s="47">
-        <v>44685.666666666664</v>
+        <v>44683.375</v>
       </c>
       <c r="L1366" s="46">
-        <f t="shared" si="52"/>
-        <v>1651680000000</v>
+        <f t="shared" si="53"/>
+        <v>1651482000000</v>
       </c>
     </row>
     <row r="1367">
       <c r="A1367" s="1">
-        <v>1307.0</v>
+        <v>1303.0</v>
       </c>
       <c r="B1367" s="1" t="s">
         <v>749</v>
       </c>
       <c r="C1367" s="1" t="s">
-        <v>34</v>
+        <v>2183</v>
       </c>
       <c r="D1367" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K1367" s="47">
-        <v>44686.5</v>
+        <v>44683.541666666664</v>
       </c>
       <c r="L1367" s="46">
-        <f t="shared" si="52"/>
-        <v>1651752000000</v>
+        <f t="shared" si="53"/>
+        <v>1651496400000</v>
       </c>
     </row>
     <row r="1368">
       <c r="A1368" s="1">
-        <v>1308.0</v>
+        <v>1305.0</v>
       </c>
       <c r="B1368" s="1" t="s">
         <v>749</v>
       </c>
       <c r="C1368" s="1" t="s">
+        <v>2184</v>
+      </c>
+      <c r="D1368" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K1368" s="47">
+        <v>44685.458333333336</v>
+      </c>
+      <c r="L1368" s="46">
+        <f t="shared" si="53"/>
+        <v>1651662000000</v>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" s="1">
+        <v>1306.0</v>
+      </c>
+      <c r="B1369" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C1369" s="1" t="s">
+        <v>2185</v>
+      </c>
+      <c r="D1369" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K1369" s="47">
+        <v>44685.666666666664</v>
+      </c>
+      <c r="L1369" s="46">
+        <f t="shared" si="53"/>
+        <v>1651680000000</v>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" s="1">
+        <v>1307.0</v>
+      </c>
+      <c r="B1370" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C1370" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1370" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K1370" s="47">
+        <v>44686.5</v>
+      </c>
+      <c r="L1370" s="46">
+        <f t="shared" si="53"/>
+        <v>1651752000000</v>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" s="1">
+        <v>1308.0</v>
+      </c>
+      <c r="B1371" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C1371" s="1" t="s">
         <v>2186</v>
       </c>
-      <c r="D1368" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K1368" s="47">
+      <c r="D1371" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K1371" s="47">
         <v>44687.125</v>
       </c>
-      <c r="L1368" s="46">
-        <f t="shared" si="52"/>
+      <c r="L1371" s="46">
+        <f t="shared" si="53"/>
         <v>1651806000000</v>
       </c>
     </row>
-    <row r="1369">
-      <c r="A1369" s="1"/>
-      <c r="B1369" s="1" t="s">
+    <row r="1372">
+      <c r="A1372" s="1"/>
+      <c r="B1372" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C1369" s="1"/>
-      <c r="D1369" s="1"/>
-      <c r="K1369" s="47"/>
-      <c r="L1369" s="46"/>
-      <c r="M1369" s="1">
+      <c r="C1372" s="1"/>
+      <c r="D1372" s="1"/>
+      <c r="K1372" s="47"/>
+      <c r="L1372" s="46"/>
+      <c r="M1372" s="1">
         <v>1308.0</v>
       </c>
     </row>
-    <row r="1370">
-      <c r="A1370" s="1"/>
-      <c r="B1370" s="1" t="s">
+    <row r="1373">
+      <c r="A1373" s="1"/>
+      <c r="B1373" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C1370" s="1"/>
-      <c r="D1370" s="1"/>
-      <c r="K1370" s="47"/>
-      <c r="L1370" s="46"/>
-      <c r="M1370" s="1">
+      <c r="C1373" s="1"/>
+      <c r="D1373" s="1"/>
+      <c r="K1373" s="47"/>
+      <c r="L1373" s="46"/>
+      <c r="M1373" s="1">
         <v>1308.0</v>
       </c>
     </row>
-    <row r="1371">
-      <c r="A1371" s="1"/>
-      <c r="B1371" s="1" t="s">
+    <row r="1374">
+      <c r="A1374" s="1"/>
+      <c r="B1374" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C1371" s="1"/>
-      <c r="D1371" s="1"/>
-      <c r="K1371" s="47"/>
-      <c r="L1371" s="46"/>
-      <c r="M1371" s="1">
+      <c r="C1374" s="1"/>
+      <c r="D1374" s="1"/>
+      <c r="K1374" s="47"/>
+      <c r="L1374" s="46"/>
+      <c r="M1374" s="1">
         <v>1308.0</v>
       </c>
     </row>
-    <row r="1372">
-      <c r="A1372" s="1">
+    <row r="1375">
+      <c r="A1375" s="1">
         <v>1309.0</v>
       </c>
-      <c r="B1372" s="1" t="s">
+      <c r="B1375" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="C1372" s="1" t="s">
+      <c r="C1375" s="1" t="s">
         <v>2187</v>
       </c>
-      <c r="D1372" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K1372" s="47">
+      <c r="D1375" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K1375" s="47">
         <v>44687.5</v>
       </c>
-      <c r="L1372" s="46">
-        <f t="shared" ref="L1372:L1374" si="53">(K1372-Date(1970,1,1))*86400*1000</f>
+      <c r="L1375" s="46">
+        <f t="shared" ref="L1375:L1377" si="54">(K1375-Date(1970,1,1))*86400*1000</f>
         <v>1651838400000</v>
       </c>
     </row>
-    <row r="1373">
-      <c r="A1373" s="1">
+    <row r="1376">
+      <c r="A1376" s="1">
         <v>1310.0</v>
       </c>
-      <c r="B1373" s="1" t="s">
+      <c r="B1376" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="C1373" s="1" t="s">
+      <c r="C1376" s="1" t="s">
         <v>2188</v>
       </c>
-      <c r="D1373" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K1373" s="47">
+      <c r="D1376" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K1376" s="47">
         <v>44688.5</v>
       </c>
-      <c r="L1373" s="46">
-        <f t="shared" si="53"/>
+      <c r="L1376" s="46">
+        <f t="shared" si="54"/>
         <v>1651924800000</v>
       </c>
     </row>
-    <row r="1374">
-      <c r="A1374" s="1">
+    <row r="1377">
+      <c r="A1377" s="1">
         <v>1311.0</v>
       </c>
-      <c r="B1374" s="1" t="s">
+      <c r="B1377" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="C1374" s="1" t="s">
+      <c r="C1377" s="1" t="s">
         <v>1703</v>
       </c>
-      <c r="D1374" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K1374" s="47">
+      <c r="D1377" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K1377" s="47">
         <v>44689.5</v>
       </c>
-      <c r="L1374" s="46">
-        <f t="shared" si="53"/>
+      <c r="L1377" s="46">
+        <f t="shared" si="54"/>
         <v>1652011200000</v>
       </c>
     </row>
@@ -40589,15 +40628,15 @@
     <hyperlink r:id="rId1051" ref="E1334"/>
     <hyperlink r:id="rId1052" ref="E1335"/>
     <hyperlink r:id="rId1053" ref="E1336"/>
-    <hyperlink r:id="rId1054" ref="E1343"/>
-    <hyperlink r:id="rId1055" ref="E1344"/>
-    <hyperlink r:id="rId1056" ref="E1345"/>
-    <hyperlink r:id="rId1057" ref="E1351"/>
-    <hyperlink r:id="rId1058" ref="E1352"/>
-    <hyperlink r:id="rId1059" ref="E1358"/>
-    <hyperlink r:id="rId1060" ref="E1360"/>
-    <hyperlink r:id="rId1061" ref="E1362"/>
-    <hyperlink r:id="rId1062" ref="E1363"/>
+    <hyperlink r:id="rId1054" ref="E1346"/>
+    <hyperlink r:id="rId1055" ref="E1347"/>
+    <hyperlink r:id="rId1056" ref="E1348"/>
+    <hyperlink r:id="rId1057" ref="E1354"/>
+    <hyperlink r:id="rId1058" ref="E1355"/>
+    <hyperlink r:id="rId1059" ref="E1361"/>
+    <hyperlink r:id="rId1060" ref="E1363"/>
+    <hyperlink r:id="rId1061" ref="E1365"/>
+    <hyperlink r:id="rId1062" ref="E1366"/>
   </hyperlinks>
   <drawing r:id="rId1063"/>
 </worksheet>

</xml_diff>